<commit_message>
fix: Add bugfix concerning the partial overlap with some specific dbVar SV (same start and end locations) (v3.2.1)
</commit_message>
<xml_diff>
--- a/Scoring_Criteria_AnnotSV_v3.2.xlsx
+++ b/Scoring_Criteria_AnnotSV_v3.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veron\Desktop\Tutu\AnnotSV ranking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226436EA-EC35-4450-8C9C-4E4D3A0EC505}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F17607-CB0B-4788-A121-D6CB7FF51985}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="3615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1797,12 +1797,6 @@
     </r>
   </si>
   <si>
-    <t>Table 2: AnnotSV (v3.1.4) implementation of the Gain CNV interpretation scoring metric</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">2B. </t>
     </r>
@@ -1868,6 +1862,12 @@
   </si>
   <si>
     <t>po_B_gain_someG_coord</t>
+  </si>
+  <si>
+    <t>Table 2: AnnotSV (v3.2) implementation of the Gain CNV interpretation scoring metric</t>
+  </si>
+  <si>
+    <t>Table 1: AnnotSV (v3.2) implementation of the Loss CNV interpretation scoring metric</t>
   </si>
 </sst>
 </file>
@@ -2609,6 +2609,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2645,6 +2669,15 @@
     <xf numFmtId="0" fontId="29" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2657,11 +2690,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2696,6 +2741,12 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2703,57 +2754,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2994,7 +2994,7 @@
   <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:B66"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3007,29 +3007,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="61" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="63"/>
+      <c r="A1" s="69" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="72" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74"/>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="A3" s="75"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
@@ -3049,13 +3049,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
@@ -3090,13 +3090,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
     </row>
     <row r="9" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
@@ -3116,46 +3116,46 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="78"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="57" t="s">
-        <v>173</v>
-      </c>
-      <c r="C10" s="105">
+        <v>171</v>
+      </c>
+      <c r="C10" s="67">
         <v>0</v>
       </c>
-      <c r="D10" s="105" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="106" t="s">
-        <v>178</v>
+      <c r="D10" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="81" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="107"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="82"/>
     </row>
     <row r="12" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="78"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
-      <c r="E12" s="107"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="82"/>
     </row>
     <row r="13" spans="1:5" s="58" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="108"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
@@ -3362,14 +3362,14 @@
       <c r="B28" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="109">
+      <c r="C28" s="64">
         <v>0</v>
       </c>
-      <c r="D28" s="109" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="103" t="s">
-        <v>174</v>
+      <c r="D28" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="E28" s="63" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3390,13 +3390,13 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
     </row>
     <row r="31" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -3446,16 +3446,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
     </row>
     <row r="35" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="79" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="30" t="s">
@@ -3466,7 +3466,7 @@
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
+      <c r="A36" s="79"/>
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71"/>
+      <c r="A37" s="79"/>
       <c r="B37" s="30" t="s">
         <v>24</v>
       </c>
@@ -3652,24 +3652,24 @@
       <c r="B52" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="C52" s="109">
+      <c r="C52" s="64">
         <v>-1</v>
       </c>
-      <c r="D52" s="103" t="s">
-        <v>96</v>
-      </c>
-      <c r="E52" s="103" t="s">
-        <v>176</v>
+      <c r="D52" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="E52" s="63" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="70" t="s">
+      <c r="A53" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="70"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="78"/>
     </row>
     <row r="54" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="30" t="s">
@@ -3776,57 +3776,57 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="76"/>
-      <c r="B62" s="76"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="76"/>
+      <c r="A62" s="87"/>
+      <c r="B62" s="87"/>
+      <c r="C62" s="87"/>
+      <c r="D62" s="87"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="77" t="s">
+      <c r="A63" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="B63" s="77"/>
-      <c r="C63" s="77"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="77"/>
+      <c r="B63" s="65"/>
+      <c r="C63" s="65"/>
+      <c r="D63" s="65"/>
+      <c r="E63" s="65"/>
     </row>
     <row r="64" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="74" t="s">
+      <c r="A64" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="B64" s="75"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="73" t="s">
+      <c r="A65" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="73"/>
+      <c r="B65" s="84"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="104" t="s">
-        <v>175</v>
-      </c>
-      <c r="B66" s="104"/>
+      <c r="A66" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="D10:D13"/>
     <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="A34:E34"/>
@@ -3845,8 +3845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:B66"/>
+    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3859,29 +3859,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="79" t="s">
-        <v>171</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="81"/>
+      <c r="A1" s="94" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="96"/>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="97" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="84"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="88"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
+      <c r="A3" s="103"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
@@ -3901,13 +3901,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="102"/>
     </row>
     <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -3942,13 +3942,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="87"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="102"/>
     </row>
     <row r="9" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
@@ -3968,46 +3968,46 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89"/>
+      <c r="A10" s="104"/>
       <c r="B10" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="93">
+      <c r="C10" s="105">
         <v>0</v>
       </c>
-      <c r="D10" s="94" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="95" t="s">
-        <v>177</v>
+      <c r="D10" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="91" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="89"/>
+      <c r="A11" s="104"/>
       <c r="B11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="96"/>
-      <c r="D11" s="97"/>
-      <c r="E11" s="98"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="92"/>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="89"/>
+      <c r="A12" s="104"/>
       <c r="B12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="89"/>
+      <c r="E12" s="92"/>
     </row>
     <row r="13" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="89"/>
+      <c r="A13" s="104"/>
       <c r="B13" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="100"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
@@ -4022,8 +4022,8 @@
       <c r="D14" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="101" t="s">
-        <v>179</v>
+      <c r="E14" s="61" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4065,8 +4065,8 @@
       <c r="D17" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="101" t="s">
-        <v>179</v>
+      <c r="E17" s="61" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4080,8 +4080,8 @@
       <c r="D18" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="101" t="s">
-        <v>181</v>
+      <c r="E18" s="61" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4227,13 +4227,13 @@
       <c r="E28" s="36"/>
     </row>
     <row r="29" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="85" t="s">
+      <c r="A29" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="86"/>
-      <c r="C29" s="86"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="87"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="102"/>
     </row>
     <row r="30" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
@@ -4283,16 +4283,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="100" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="86"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="86"/>
-      <c r="E33" s="87"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
+      <c r="E33" s="102"/>
     </row>
     <row r="34" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="91" t="s">
+      <c r="A34" s="108" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="17" t="s">
@@ -4303,7 +4303,7 @@
       <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="91"/>
+      <c r="A35" s="108"/>
       <c r="B35" s="17" t="s">
         <v>69</v>
       </c>
@@ -4312,7 +4312,7 @@
       <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="91"/>
+      <c r="A36" s="108"/>
       <c r="B36" s="16" t="s">
         <v>70</v>
       </c>
@@ -4486,7 +4486,7 @@
     </row>
     <row r="51" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="62" t="s">
         <v>84</v>
       </c>
       <c r="C51" s="49">
@@ -4495,18 +4495,18 @@
       <c r="D51" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="103" t="s">
-        <v>180</v>
+      <c r="E51" s="63" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="85" t="s">
+      <c r="A52" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="86"/>
-      <c r="C52" s="86"/>
-      <c r="D52" s="86"/>
-      <c r="E52" s="87"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="102"/>
     </row>
     <row r="53" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
@@ -4613,64 +4613,59 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="92"/>
-      <c r="B61" s="92"/>
-      <c r="C61" s="92"/>
+      <c r="A61" s="109"/>
+      <c r="B61" s="109"/>
+      <c r="C61" s="109"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
     <row r="62" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="77" t="s">
+      <c r="A62" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="B62" s="77"/>
-      <c r="C62" s="77"/>
-      <c r="D62" s="77"/>
-      <c r="E62" s="77"/>
+      <c r="B62" s="65"/>
+      <c r="C62" s="65"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
     </row>
     <row r="63" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="74" t="s">
+      <c r="A63" s="85" t="s">
         <v>167</v>
       </c>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
+      <c r="B63" s="86"/>
+      <c r="C63" s="86"/>
+      <c r="D63" s="86"/>
+      <c r="E63" s="86"/>
     </row>
     <row r="64" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="74" t="s">
+      <c r="A64" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="B64" s="75"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
+      <c r="B64" s="86"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="73" t="s">
+      <c r="A65" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="B65" s="73"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="73"/>
+      <c r="B65" s="84"/>
+      <c r="C65" s="84"/>
+      <c r="D65" s="84"/>
+      <c r="E65" s="84"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="104" t="s">
-        <v>175</v>
-      </c>
-      <c r="B66" s="104"/>
+      <c r="A66" s="68" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="68"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="A65:E65"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A5:E5"/>
@@ -4685,6 +4680,11 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A52:E52"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A65:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>